<commit_message>
2017-18 common variables data
</commit_message>
<xml_diff>
--- a/data/CO/2017-2018/2017-18 Average Salaries for Teachers.xlsx
+++ b/data/CO/2017-2018/2017-18 Average Salaries for Teachers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Data Services\Statistics Web Page\2017-18 Staff Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishikth\Downloads\ds 5110 dataset\additional\2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,21 +32,6 @@
     <t>2017-2018 TEACHERS FTE AND AVERAGE SALARY</t>
   </si>
   <si>
-    <t>School Year</t>
-  </si>
-  <si>
-    <t>Organization Code</t>
-  </si>
-  <si>
-    <t>Orgnazation Name</t>
-  </si>
-  <si>
-    <t>Total FTE</t>
-  </si>
-  <si>
-    <t>Average Salary</t>
-  </si>
-  <si>
     <t>2017-2018</t>
   </si>
   <si>
@@ -1227,6 +1212,21 @@
   </si>
   <si>
     <t>2017-2018 Total</t>
+  </si>
+  <si>
+    <t>Organization_Code</t>
+  </si>
+  <si>
+    <t>Orgnazation_Name</t>
+  </si>
+  <si>
+    <t>Average_Salary</t>
+  </si>
+  <si>
+    <t>School_Year</t>
+  </si>
+  <si>
+    <t>Total_FTE</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1597,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1631,30 +1631,30 @@
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>399</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>396</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>397</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>400</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
         <v>358.47120000000001</v>
@@ -1665,13 +1665,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5">
         <v>1969.8787000000118</v>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5">
         <v>376.35090000000014</v>
@@ -1699,13 +1699,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5">
         <v>793.9368999999989</v>
@@ -1716,13 +1716,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D9" s="5">
         <v>62.222200000000001</v>
@@ -1733,13 +1733,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D10" s="5">
         <v>60.9694</v>
@@ -1750,13 +1750,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5">
         <v>521.80819999999949</v>
@@ -1767,13 +1767,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5">
         <v>129.80560000000003</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5">
         <v>26.214499999999997</v>
@@ -1801,13 +1801,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5">
         <v>184.1506999999998</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5">
         <v>99.866300000000024</v>
@@ -1835,13 +1835,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5">
         <v>3110.2273000000059</v>
@@ -1852,13 +1852,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5">
         <v>835.13869999999963</v>
@@ -1869,13 +1869,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18" s="5">
         <v>17.845800000000001</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5">
         <v>2154.0317000000164</v>
@@ -1903,13 +1903,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5">
         <v>80.636100000000084</v>
@@ -1920,13 +1920,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5">
         <v>99.586699999999979</v>
@@ -1937,13 +1937,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5">
         <v>15.8766</v>
@@ -1954,13 +1954,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5">
         <v>7.6150000000000011</v>
@@ -1971,13 +1971,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5">
         <v>28.362500000000001</v>
@@ -1988,13 +1988,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D25" s="5">
         <v>7.625</v>
@@ -2005,13 +2005,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D26" s="5">
         <v>8.9435000000000002</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D27" s="5">
         <v>42.236599999999989</v>
@@ -2039,13 +2039,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D28" s="5">
         <v>20.732399999999998</v>
@@ -2056,13 +2056,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D29" s="5">
         <v>1783.446300000001</v>
@@ -2073,13 +2073,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D30" s="5">
         <v>1716.8948000000023</v>
@@ -2090,13 +2090,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D31" s="5">
         <v>73.9375</v>
@@ -2107,13 +2107,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D32" s="5">
         <v>92.224499999999978</v>
@@ -2124,13 +2124,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D33" s="5">
         <v>15.060300000000002</v>
@@ -2141,13 +2141,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D34" s="5">
         <v>17.247300000000003</v>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D35" s="5">
         <v>57.058900000000001</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D36" s="5">
         <v>70.701699999999988</v>
@@ -2192,13 +2192,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D37" s="5">
         <v>25.348599999999998</v>
@@ -2209,13 +2209,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D38" s="5">
         <v>18.503300000000003</v>
@@ -2226,13 +2226,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D39" s="5">
         <v>20.3126</v>
@@ -2243,13 +2243,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D40" s="5">
         <v>21.995199999999997</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D41" s="5">
         <v>31.170400000000004</v>
@@ -2277,13 +2277,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D42" s="5">
         <v>25.649099999999997</v>
@@ -2294,13 +2294,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D43" s="5">
         <v>282.82809999999989</v>
@@ -2311,13 +2311,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D44" s="5">
         <v>6109.7128000000275</v>
@@ -2328,13 +2328,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D45" s="5">
         <v>19.456900000000001</v>
@@ -2345,13 +2345,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D46" s="5">
         <v>3526.564299999995</v>
@@ -2362,13 +2362,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D47" s="5">
         <v>469.97590000000031</v>
@@ -2379,13 +2379,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D48" s="5">
         <v>143.9325</v>
@@ -2396,13 +2396,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D49" s="5">
         <v>21.75</v>
@@ -2413,13 +2413,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D50" s="5">
         <v>26.023700000000005</v>
@@ -2430,13 +2430,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D51" s="5">
         <v>20.583600000000004</v>
@@ -2447,13 +2447,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D52" s="5">
         <v>2.125</v>
@@ -2464,13 +2464,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D53" s="5">
         <v>28.099000000000004</v>
@@ -2481,13 +2481,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D54" s="5">
         <v>734.87140000000056</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D55" s="5">
         <v>547.774</v>
@@ -2515,13 +2515,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D56" s="5">
         <v>500.94280000000003</v>
@@ -2532,13 +2532,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D57" s="5">
         <v>1641.2701999999965</v>
@@ -2549,13 +2549,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D58" s="5">
         <v>353.43629999999985</v>
@@ -2566,13 +2566,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D59" s="5">
         <v>99.372100000000017</v>
@@ -2583,13 +2583,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D60" s="5">
         <v>1533.0124000000046</v>
@@ -2600,13 +2600,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D61" s="5">
         <v>67.54770000000002</v>
@@ -2617,13 +2617,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D62" s="5">
         <v>39.144600000000011</v>
@@ -2634,13 +2634,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D63" s="5">
         <v>21.596900000000002</v>
@@ -2651,13 +2651,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D64" s="5">
         <v>368.21670000000017</v>
@@ -2668,13 +2668,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D65" s="5">
         <v>1048.2109000000023</v>
@@ -2685,13 +2685,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D66" s="5">
         <v>14.822799999999999</v>
@@ -2702,13 +2702,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D67" s="5">
         <v>21.031400000000005</v>
@@ -2719,13 +2719,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D68" s="5">
         <v>227.38610000000003</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D69" s="5">
         <v>93.536500000000004</v>
@@ -2753,13 +2753,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D70" s="5">
         <v>19.680600000000005</v>
@@ -2770,13 +2770,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D71" s="5">
         <v>379.89019999999988</v>
@@ -2787,13 +2787,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D72" s="5">
         <v>284.08170000000013</v>
@@ -2804,13 +2804,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D73" s="5">
         <v>76.205199999999991</v>
@@ -2821,13 +2821,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D74" s="5">
         <v>34.973199999999991</v>
@@ -2838,13 +2838,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D75" s="5">
         <v>38.180700000000002</v>
@@ -2855,13 +2855,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D76" s="5">
         <v>94</v>
@@ -2872,13 +2872,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D77" s="5">
         <v>137.3289</v>
@@ -2889,13 +2889,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D78" s="5">
         <v>12.877400000000005</v>
@@ -2906,13 +2906,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D79" s="5">
         <v>28.611000000000004</v>
@@ -2923,13 +2923,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D80" s="5">
         <v>20.942</v>
@@ -2940,13 +2940,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D81" s="5">
         <v>20.538399999999996</v>
@@ -2957,13 +2957,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D82" s="5">
         <v>4690.4733999999444</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D83" s="5">
         <v>17.448700000000002</v>
@@ -2991,13 +2991,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D84" s="5">
         <v>8.7110000000000003</v>
@@ -3008,13 +3008,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D85" s="5">
         <v>16.915500000000002</v>
@@ -3025,13 +3025,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D86" s="5">
         <v>13.9452</v>
@@ -3042,13 +3042,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C87" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D87" s="5">
         <v>17.546299999999999</v>
@@ -3059,13 +3059,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C88" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D88" s="5">
         <v>13.266500000000002</v>
@@ -3076,13 +3076,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C89" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D89" s="5">
         <v>49.156300000000002</v>
@@ -3093,13 +3093,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D90" s="5">
         <v>61.25</v>
@@ -3110,13 +3110,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D91" s="5">
         <v>383.20519999999999</v>
@@ -3127,13 +3127,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D92" s="5">
         <v>76.499099999999999</v>
@@ -3144,13 +3144,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D93" s="5">
         <v>66.75</v>
@@ -3161,13 +3161,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D94" s="5">
         <v>1743.7638000000004</v>
@@ -3178,13 +3178,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C95" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D95" s="5">
         <v>910.20039999999949</v>
@@ -3195,13 +3195,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C96" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D96" s="5">
         <v>76.798200000000008</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C97" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D97" s="5">
         <v>57.049399999999999</v>
@@ -3229,13 +3229,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D98" s="5">
         <v>20.665300000000002</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D99" s="5">
         <v>21.850100000000005</v>
@@ -3263,13 +3263,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D100" s="5">
         <v>11.55</v>
@@ -3280,13 +3280,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D101" s="5">
         <v>31.1981</v>
@@ -3297,13 +3297,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D102" s="5">
         <v>9.8467000000000002</v>
@@ -3314,13 +3314,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C103" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D103" s="5">
         <v>18</v>
@@ -3331,13 +3331,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C104" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D104" s="5">
         <v>32.821600000000004</v>
@@ -3348,13 +3348,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D105" s="5">
         <v>6.5956000000000001</v>
@@ -3365,13 +3365,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D106" s="5">
         <v>139.13500000000002</v>
@@ -3382,13 +3382,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C107" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D107" s="5">
         <v>20.8308</v>
@@ -3399,13 +3399,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C108" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D108" s="5">
         <v>21.087599999999998</v>
@@ -3416,13 +3416,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D109" s="5">
         <v>16.3489</v>
@@ -3433,13 +3433,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D110" s="5">
         <v>18.059000000000001</v>
@@ -3450,13 +3450,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D111" s="5">
         <v>27.7818</v>
@@ -3467,13 +3467,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C112" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D112" s="5">
         <v>1280.4928000000002</v>
@@ -3484,13 +3484,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C113" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D113" s="5">
         <v>10.954699999999999</v>
@@ -3501,13 +3501,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D114" s="5">
         <v>126.65989999999996</v>
@@ -3518,13 +3518,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C115" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D115" s="5">
         <v>176.62990000000005</v>
@@ -3535,13 +3535,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D116" s="5">
         <v>50.966500000000003</v>
@@ -3552,13 +3552,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D117" s="5">
         <v>31.204800000000002</v>
@@ -3569,13 +3569,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D118" s="5">
         <v>335.44470000000013</v>
@@ -3586,13 +3586,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C119" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D119" s="5">
         <v>24.539300000000004</v>
@@ -3603,13 +3603,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B120" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D120" s="5">
         <v>97.37700000000001</v>
@@ -3620,13 +3620,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C121" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D121" s="5">
         <v>200.17449999999999</v>
@@ -3637,13 +3637,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C122" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D122" s="5">
         <v>17.752800000000001</v>
@@ -3654,13 +3654,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C123" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D123" s="5">
         <v>35.968699999999998</v>
@@ -3671,13 +3671,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C124" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D124" s="5">
         <v>89.967399999999998</v>
@@ -3688,13 +3688,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D125" s="5">
         <v>59.433399999999999</v>
@@ -3705,13 +3705,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C126" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D126" s="5">
         <v>16.2</v>
@@ -3722,13 +3722,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C127" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D127" s="5">
         <v>34.919899999999991</v>
@@ -3739,13 +3739,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B128" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C128" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D128" s="5">
         <v>17.061</v>
@@ -3756,13 +3756,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C129" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D129" s="5">
         <v>28.1843</v>
@@ -3773,13 +3773,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C130" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D130" s="5">
         <v>22.731400000000001</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C131" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D131" s="5">
         <v>29.9068</v>
@@ -3807,13 +3807,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C132" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D132" s="5">
         <v>57.435400000000016</v>
@@ -3824,13 +3824,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C133" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D133" s="5">
         <v>44.195899999999995</v>
@@ -3841,13 +3841,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C134" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D134" s="5">
         <v>47.494599999999998</v>
@@ -3858,13 +3858,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B135" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C135" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D135" s="5">
         <v>24.598399999999998</v>
@@ -3875,13 +3875,13 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C136" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D136" s="5">
         <v>141.14570000000001</v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D137" s="5">
         <v>16.584099999999999</v>
@@ -3909,13 +3909,13 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C138" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D138" s="5">
         <v>104.00560000000002</v>
@@ -3926,13 +3926,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C139" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D139" s="5">
         <v>23.1389</v>
@@ -3943,13 +3943,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C140" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D140" s="5">
         <v>22.933800000000002</v>
@@ -3960,13 +3960,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C141" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D141" s="5">
         <v>1003.8707000000015</v>
@@ -3977,13 +3977,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C142" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D142" s="5">
         <v>507.27020000000022</v>
@@ -3994,13 +3994,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C143" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D143" s="5">
         <v>43.0625</v>
@@ -4011,13 +4011,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C144" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D144" s="5">
         <v>32.343899999999998</v>
@@ -4028,13 +4028,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C145" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D145" s="5">
         <v>28.213100000000004</v>
@@ -4045,13 +4045,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B146" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C146" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D146" s="5">
         <v>76.2864</v>
@@ -4062,13 +4062,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B147" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C147" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D147" s="5">
         <v>28.556999999999999</v>
@@ -4079,13 +4079,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B148" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C148" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D148" s="5">
         <v>33.718299999999999</v>
@@ -4096,13 +4096,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B149" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C149" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D149" s="5">
         <v>163.54550000000006</v>
@@ -4113,13 +4113,13 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C150" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D150" s="5">
         <v>30.6675</v>
@@ -4130,13 +4130,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C151" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D151" s="5">
         <v>14.513400000000001</v>
@@ -4147,13 +4147,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C152" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D152" s="5">
         <v>21.871700000000001</v>
@@ -4164,13 +4164,13 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C153" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D153" s="5">
         <v>45.693600000000004</v>
@@ -4181,13 +4181,13 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B154" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C154" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D154" s="5">
         <v>10.7653</v>
@@ -4198,13 +4198,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C155" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D155" s="5">
         <v>74.723900000000029</v>
@@ -4215,13 +4215,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C156" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D156" s="5">
         <v>18.375</v>
@@ -4232,13 +4232,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C157" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D157" s="5">
         <v>34.250599999999991</v>
@@ -4249,13 +4249,13 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C158" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D158" s="5">
         <v>14.785800000000002</v>
@@ -4266,13 +4266,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C159" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D159" s="5">
         <v>248.95939999999996</v>
@@ -4283,13 +4283,13 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C160" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D160" s="5">
         <v>28.235299999999999</v>
@@ -4300,13 +4300,13 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C161" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D161" s="5">
         <v>142.68879999999996</v>
@@ -4317,13 +4317,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C162" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D162" s="5">
         <v>32.521599999999992</v>
@@ -4334,13 +4334,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C163" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D163" s="5">
         <v>13.348099999999999</v>
@@ -4351,13 +4351,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C164" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D164" s="5">
         <v>18.491500000000002</v>
@@ -4368,13 +4368,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B165" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C165" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D165" s="5">
         <v>17.894900000000007</v>
@@ -4385,13 +4385,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B166" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C166" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D166" s="5">
         <v>11.025300000000001</v>
@@ -4402,13 +4402,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B167" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C167" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D167" s="5">
         <v>137.71509999999998</v>
@@ -4419,13 +4419,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B168" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C168" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D168" s="5">
         <v>115.1288</v>
@@ -4436,13 +4436,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B169" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C169" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D169" s="5">
         <v>146.22460000000004</v>
@@ -4453,13 +4453,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B170" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C170" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D170" s="5">
         <v>351.46779999999973</v>
@@ -4470,13 +4470,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B171" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C171" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D171" s="5">
         <v>194.45670000000001</v>
@@ -4487,13 +4487,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B172" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C172" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D172" s="5">
         <v>1228.0757000000008</v>
@@ -4504,13 +4504,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B173" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C173" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D173" s="5">
         <v>81.498700000000014</v>
@@ -4521,13 +4521,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B174" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C174" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D174" s="5">
         <v>141.67679999999996</v>
@@ -4538,13 +4538,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B175" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C175" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D175" s="5">
         <v>62.510999999999989</v>
@@ -4555,13 +4555,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B176" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C176" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D176" s="5">
         <v>18.921700000000001</v>
@@ -4572,13 +4572,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B177" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C177" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D177" s="5">
         <v>17.290400000000002</v>
@@ -4589,13 +4589,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B178" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C178" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D178" s="5">
         <v>16.864700000000006</v>
@@ -4606,13 +4606,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B179" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C179" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D179" s="5">
         <v>64.214399999999998</v>
@@ -4623,13 +4623,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B180" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C180" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D180" s="5">
         <v>53.822600000000008</v>
@@ -4640,13 +4640,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B181" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C181" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D181" s="5">
         <v>16.139600000000002</v>
@@ -4657,13 +4657,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B182" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C182" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D182" s="5">
         <v>10.1388</v>
@@ -4674,13 +4674,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B183" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C183" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D183" s="5">
         <v>906.97659999999644</v>
@@ -4691,13 +4691,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B184" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C184" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D184" s="5">
         <v>36.77109999999999</v>
@@ -4708,13 +4708,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B185" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C185" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D185" s="5">
         <v>7.8631999999999991</v>
@@ -4725,13 +4725,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B186" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C186" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D186" s="5">
         <v>0.6520999999999999</v>
@@ -4742,13 +4742,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B187" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C187" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D187" s="5">
         <v>19.109500000000004</v>
@@ -4759,13 +4759,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B188" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C188" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D188" s="5">
         <v>2.5794000000000001</v>
@@ -4776,13 +4776,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B189" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C189" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D189" s="5">
         <v>20.562999999999999</v>
@@ -4793,13 +4793,13 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B190" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C190" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D190" s="5">
         <v>3.9974999999999996</v>
@@ -4810,13 +4810,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B191" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C191" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D191" s="5">
         <v>14.727</v>
@@ -4827,13 +4827,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B192" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C192" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D192" s="5">
         <v>4.4999000000000002</v>
@@ -4844,13 +4844,13 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C193" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D193" s="5">
         <v>0.99379999999999991</v>
@@ -4861,13 +4861,13 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B194" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C194" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D194" s="5">
         <v>5.9499999999999993</v>
@@ -4878,13 +4878,13 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B195" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C195" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D195" s="5">
         <v>29.294799999999981</v>
@@ -4895,13 +4895,13 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B196" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C196" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D196" s="5">
         <v>0.64270000000000005</v>
@@ -4912,13 +4912,13 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B197" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C197" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D197" s="5">
         <v>3.6976999999999993</v>
@@ -4929,13 +4929,13 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C198" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D198" s="5">
         <v>1.9358</v>
@@ -4946,13 +4946,13 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B199" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C199" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D199" s="5">
         <v>61.5</v>
@@ -4963,13 +4963,13 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B200" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C200" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D200" s="5">
         <v>14.019299999999998</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D201" s="5">
         <v>52347.068700000003</v>

</xml_diff>